<commit_message>
CIARegister 0 and 1 small improvement.
</commit_message>
<xml_diff>
--- a/docs/C64Data/CIA1Logic.xlsx
+++ b/docs/C64Data/CIA1Logic.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\C64Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B266F4FB-DEAC-4D35-9743-E1F2946CE1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39F19F0-060F-4F24-8081-9A645D672197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="1" xr2:uid="{FAE2CC58-5876-4D28-B475-9361A6F1250D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{FAE2CC58-5876-4D28-B475-9361A6F1250D}"/>
   </bookViews>
   <sheets>
     <sheet name="Port Behaviour" sheetId="2" r:id="rId1"/>
     <sheet name="Process" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -318,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -344,9 +343,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BD1EBF-4660-49B3-BAB2-7E4CF41FCD70}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -751,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDF2AD0-948E-4A7A-BE59-5B781662EEF9}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -993,7 +989,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1010,7 +1006,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="2" t="s">

</xml_diff>